<commit_message>
the build is running again
</commit_message>
<xml_diff>
--- a/data/sample_survey_export.xlsx
+++ b/data/sample_survey_export.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLuedtke\ACM-School-Placement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perus\GitHub\ACM-School-Placement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B486A777-4620-4D65-B19A-9FA883A6AA3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8796"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20170616172952-SurveyExport" sheetId="1" r:id="rId1"/>
@@ -534,7 +535,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1336,16 +1337,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="106.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="118.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="63.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="70.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="56.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="72.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="56.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="67.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="75.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="90.36328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="86.7265625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="85.54296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="59.90625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="56.1796875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="54.08984375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="47.90625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="68.90625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="61.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="80.81640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="60" width="56.7265625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="33.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1530,7 +1587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1544,7 +1601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1624,7 +1681,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1722,7 +1779,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1775,7 +1832,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1897,7 +1954,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1974,7 +2031,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2066,7 +2123,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2185,7 +2242,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2310,7 +2367,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2384,7 +2441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2470,7 +2527,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2484,7 +2541,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2540,7 +2597,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2608,7 +2665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2622,7 +2679,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>19</v>
       </c>
@@ -2684,7 +2741,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20</v>
       </c>

</xml_diff>